<commit_message>
update for resutls page
</commit_message>
<xml_diff>
--- a/docs/ORIGINAL.xlsx
+++ b/docs/ORIGINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jvarela/Development/github/nutreconelalma_v2.2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A268E9A8-C3B6-F94F-8443-C44CCF7E7592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326513AC-9E0F-7F41-B86A-605312E1EB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21360" yWindow="520" windowWidth="25200" windowHeight="25260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metodo 1 (2)" sheetId="7" r:id="rId1"/>
@@ -41,6 +41,49 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Joseph Varela Badilla</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{5428ACF5-C60F-9344-AC51-74FCB86E9C97}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Joseph Varela Badilla:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>la variable "cantidad" hace falta!!!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="226">
   <si>
@@ -774,7 +817,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
@@ -784,8 +827,9 @@
     <numFmt numFmtId="170" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="_-[$COP]\ * #,##0.0_-;\-[$COP]\ * #,##0.0_-;_-[$COP]\ * &quot;-&quot;?_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.0000000"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.00\ [$COP]_-;\-* #,##0.00\ [$COP]_-;_-* &quot;-&quot;??\ [$COP]_-;_-@_-"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,6 +1029,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1283,7 +1340,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1445,24 +1502,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1482,6 +1521,29 @@
     <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="22" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Accent5" xfId="5" builtinId="45"/>
@@ -1798,11 +1860,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F3DEE-FEFC-AE44-A2DE-BE929C614C50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275F3DEE-FEFC-AE44-A2DE-BE929C614C50}">
   <dimension ref="A2:X325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1811,7 +1873,7 @@
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.83203125" customWidth="1"/>
     <col min="6" max="6" width="23.83203125" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
@@ -1869,7 +1931,7 @@
       <c r="A8" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="154">
         <f>X53*T29</f>
         <v>184607</v>
       </c>
@@ -1878,7 +1940,7 @@
       <c r="A9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="154">
         <f>O52*K29</f>
         <v>86200</v>
       </c>
@@ -1887,7 +1949,7 @@
       <c r="A10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="154">
         <f>G51*C29</f>
         <v>0</v>
       </c>
@@ -1896,7 +1958,7 @@
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="155">
         <f>D63</f>
         <v>13400</v>
       </c>
@@ -1905,7 +1967,7 @@
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="155">
         <f>D74</f>
         <v>1627.395</v>
       </c>
@@ -1918,7 +1980,7 @@
       <c r="A13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="155">
         <f>D152</f>
         <v>7723.958333333333</v>
       </c>
@@ -1937,7 +1999,7 @@
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="155">
         <f>C131</f>
         <v>11680.992416666668</v>
       </c>
@@ -1953,7 +2015,7 @@
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="155">
         <f>D95</f>
         <v>32425</v>
       </c>
@@ -1964,12 +2026,15 @@
         <v>33</v>
       </c>
       <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="154"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="155">
         <f>0.36</f>
         <v>0.36</v>
       </c>
@@ -1981,7 +2046,7 @@
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="155">
         <f>+B17*B100*C119</f>
         <v>9070.434782608696</v>
       </c>
@@ -1996,7 +2061,7 @@
       <c r="A19" t="s">
         <v>202</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="155">
         <v>0.36</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -2015,7 +2080,7 @@
       <c r="A20" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="155">
         <f>+B19*G119</f>
         <v>3772.9565217391305</v>
       </c>
@@ -2029,7 +2094,7 @@
       <c r="H20" s="71"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
+      <c r="B21" s="154"/>
       <c r="F21" s="73">
         <f>B4*G15/100*G51</f>
         <v>353100</v>
@@ -2043,7 +2108,7 @@
       <c r="A22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="91">
+      <c r="B22" s="156">
         <f>+B18+B20+B11+B12+B15+B13+B14+B8</f>
         <v>264307.73705434782</v>
       </c>
@@ -4815,28 +4880,28 @@
       <c r="A126" s="115" t="s">
         <v>88</v>
       </c>
-      <c r="B126" s="118">
+      <c r="B126" s="152">
         <v>2388262</v>
       </c>
-      <c r="C126" s="118">
+      <c r="C126" s="152">
         <f>B126/$E$4/B$3</f>
         <v>1990.2183333333332</v>
       </c>
-      <c r="D126" s="129" t="s">
+      <c r="D126" s="146" t="s">
         <v>224</v>
       </c>
-      <c r="E126" s="130"/>
-      <c r="F126" s="130"/>
-      <c r="G126" s="130"/>
+      <c r="E126" s="147"/>
+      <c r="F126" s="147"/>
+      <c r="G126" s="147"/>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="B127" s="118">
+      <c r="B127" s="152">
         <v>6775276.5</v>
       </c>
-      <c r="C127" s="118">
+      <c r="C127" s="152">
         <f t="shared" ref="C127:C130" si="13">B127/$E$4/B$3</f>
         <v>5646.0637500000003</v>
       </c>
@@ -4845,10 +4910,10 @@
       <c r="A128" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="B128" s="118">
+      <c r="B128" s="152">
         <v>4783964.3999999994</v>
       </c>
-      <c r="C128" s="118">
+      <c r="C128" s="152">
         <f t="shared" si="13"/>
         <v>3986.6369999999997</v>
       </c>
@@ -4857,10 +4922,10 @@
       <c r="A129" s="115" t="s">
         <v>91</v>
       </c>
-      <c r="B129" s="118">
+      <c r="B129" s="152">
         <v>6688</v>
       </c>
-      <c r="C129" s="118">
+      <c r="C129" s="152">
         <f t="shared" si="13"/>
         <v>5.5733333333333333</v>
       </c>
@@ -4869,10 +4934,10 @@
       <c r="A130" s="115" t="s">
         <v>92</v>
       </c>
-      <c r="B130" s="118">
+      <c r="B130" s="152">
         <v>63000</v>
       </c>
-      <c r="C130" s="118">
+      <c r="C130" s="152">
         <f t="shared" si="13"/>
         <v>52.5</v>
       </c>
@@ -4882,7 +4947,7 @@
         <v>31</v>
       </c>
       <c r="B131" s="8"/>
-      <c r="C131" s="21">
+      <c r="C131" s="153">
         <f>SUM(C126:C130)</f>
         <v>11680.992416666668</v>
       </c>
@@ -5142,18 +5207,18 @@
       <c r="D154" s="34"/>
     </row>
     <row r="155" spans="1:4" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="131" t="s">
+      <c r="A155" s="148" t="s">
         <v>225</v>
       </c>
-      <c r="B155" s="131"/>
-      <c r="C155" s="131"/>
-      <c r="D155" s="131"/>
+      <c r="B155" s="148"/>
+      <c r="C155" s="148"/>
+      <c r="D155" s="148"/>
     </row>
     <row r="156" spans="1:4" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="131"/>
-      <c r="B156" s="131"/>
-      <c r="C156" s="131"/>
-      <c r="D156" s="131"/>
+      <c r="A156" s="148"/>
+      <c r="B156" s="148"/>
+      <c r="C156" s="148"/>
+      <c r="D156" s="148"/>
     </row>
     <row r="157" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="158" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -7151,131 +7216,131 @@
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A229" s="135" t="s">
+      <c r="A229" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="B229" s="136"/>
-      <c r="C229" s="136"/>
-      <c r="D229" s="136"/>
+      <c r="B229" s="130"/>
+      <c r="C229" s="130"/>
+      <c r="D229" s="130"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="136"/>
-      <c r="B230" s="136"/>
-      <c r="C230" s="136"/>
-      <c r="D230" s="136"/>
+      <c r="A230" s="130"/>
+      <c r="B230" s="130"/>
+      <c r="C230" s="130"/>
+      <c r="D230" s="130"/>
       <c r="F230" s="7"/>
     </row>
     <row r="231" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="143" t="s">
+      <c r="A231" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="B231" s="143" t="s">
+      <c r="B231" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C231" s="143" t="s">
+      <c r="C231" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D231" s="143" t="s">
+      <c r="D231" s="137" t="s">
         <v>34</v>
       </c>
       <c r="F231" s="7"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A232" s="139" t="s">
+      <c r="A232" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="B232" s="144">
-        <v>0</v>
-      </c>
-      <c r="C232" s="145">
+      <c r="B232" s="138">
+        <v>0</v>
+      </c>
+      <c r="C232" s="139">
         <v>9000</v>
       </c>
-      <c r="D232" s="139">
+      <c r="D232" s="133">
         <f>C232*B232</f>
         <v>0</v>
       </c>
       <c r="F232" s="7"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A233" s="139" t="s">
+      <c r="A233" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="B233" s="144">
-        <v>1</v>
-      </c>
-      <c r="C233" s="145">
+      <c r="B233" s="138">
+        <v>1</v>
+      </c>
+      <c r="C233" s="139">
         <v>1000</v>
       </c>
-      <c r="D233" s="139">
+      <c r="D233" s="133">
         <f t="shared" ref="D233:D236" si="33">C233*B233</f>
         <v>1000</v>
       </c>
       <c r="F233" s="7"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A234" s="139" t="s">
+      <c r="A234" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="B234" s="144">
-        <v>0</v>
-      </c>
-      <c r="C234" s="145">
+      <c r="B234" s="138">
+        <v>0</v>
+      </c>
+      <c r="C234" s="139">
         <v>1200</v>
       </c>
-      <c r="D234" s="139">
+      <c r="D234" s="133">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F234" s="7"/>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A235" s="139" t="s">
+      <c r="A235" s="133" t="s">
         <v>44</v>
       </c>
-      <c r="B235" s="144">
+      <c r="B235" s="138">
         <f>1/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C235" s="145">
+      <c r="C235" s="139">
         <v>70479</v>
       </c>
-      <c r="D235" s="139">
+      <c r="D235" s="133">
         <f t="shared" si="33"/>
         <v>352.39499999999998</v>
       </c>
       <c r="F235" s="7"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A236" s="139" t="s">
+      <c r="A236" s="133" t="s">
         <v>45</v>
       </c>
-      <c r="B236" s="144">
+      <c r="B236" s="138">
         <f>1/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C236" s="145">
+      <c r="C236" s="139">
         <v>55000</v>
       </c>
-      <c r="D236" s="139">
+      <c r="D236" s="133">
         <f t="shared" si="33"/>
         <v>275</v>
       </c>
       <c r="F236" s="7"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A237" s="136"/>
-      <c r="B237" s="148"/>
-      <c r="C237" s="136"/>
-      <c r="D237" s="136"/>
+      <c r="A237" s="130"/>
+      <c r="B237" s="142"/>
+      <c r="C237" s="130"/>
+      <c r="D237" s="130"/>
       <c r="F237" s="7"/>
     </row>
     <row r="238" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="141" t="s">
+      <c r="A238" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B238" s="151"/>
-      <c r="C238" s="141"/>
-      <c r="D238" s="151">
+      <c r="B238" s="145"/>
+      <c r="C238" s="135"/>
+      <c r="D238" s="145">
         <f>SUM(D232:D237)</f>
         <v>1627.395</v>
       </c>
@@ -7287,304 +7352,304 @@
       <c r="F239" s="7"/>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A240" s="135" t="s">
+      <c r="A240" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="B240" s="148"/>
-      <c r="C240" s="136"/>
-      <c r="D240" s="136"/>
+      <c r="B240" s="142"/>
+      <c r="C240" s="130"/>
+      <c r="D240" s="130"/>
       <c r="F240" s="7"/>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A241" s="135"/>
-      <c r="B241" s="148"/>
-      <c r="C241" s="136"/>
-      <c r="D241" s="136"/>
+      <c r="A241" s="129"/>
+      <c r="B241" s="142"/>
+      <c r="C241" s="130"/>
+      <c r="D241" s="130"/>
       <c r="F241" s="7"/>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A242" s="143" t="s">
+      <c r="A242" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="B242" s="143" t="s">
+      <c r="B242" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C242" s="143" t="s">
+      <c r="C242" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D242" s="143" t="s">
+      <c r="D242" s="137" t="s">
         <v>34</v>
       </c>
       <c r="F242" s="7"/>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A243" s="139" t="s">
+      <c r="A243" s="133" t="s">
         <v>110</v>
       </c>
-      <c r="B243" s="144">
-        <v>1</v>
-      </c>
-      <c r="C243" s="145">
+      <c r="B243" s="138">
+        <v>1</v>
+      </c>
+      <c r="C243" s="139">
         <v>400</v>
       </c>
-      <c r="D243" s="145">
+      <c r="D243" s="139">
         <f t="shared" ref="D243:D257" si="34">B243*C243</f>
         <v>400</v>
       </c>
       <c r="F243" s="7"/>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A244" s="139" t="s">
+      <c r="A244" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="B244" s="144">
-        <v>1</v>
-      </c>
-      <c r="C244" s="145">
+      <c r="B244" s="138">
+        <v>1</v>
+      </c>
+      <c r="C244" s="139">
         <v>400</v>
       </c>
-      <c r="D244" s="145">
+      <c r="D244" s="139">
         <f t="shared" si="34"/>
         <v>400</v>
       </c>
       <c r="F244" s="7"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A245" s="139" t="s">
+      <c r="A245" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="B245" s="144">
-        <v>0</v>
-      </c>
-      <c r="C245" s="145">
+      <c r="B245" s="138">
+        <v>0</v>
+      </c>
+      <c r="C245" s="139">
         <v>400</v>
       </c>
-      <c r="D245" s="145">
+      <c r="D245" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F245" s="7"/>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A246" s="139" t="s">
+      <c r="A246" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="B246" s="144">
-        <v>0</v>
-      </c>
-      <c r="C246" s="145">
+      <c r="B246" s="138">
+        <v>0</v>
+      </c>
+      <c r="C246" s="139">
         <v>500</v>
       </c>
-      <c r="D246" s="145">
+      <c r="D246" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F246" s="7"/>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A247" s="139" t="s">
+      <c r="A247" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="B247" s="144">
-        <v>1</v>
-      </c>
-      <c r="C247" s="145">
+      <c r="B247" s="138">
+        <v>1</v>
+      </c>
+      <c r="C247" s="139">
         <v>2000</v>
       </c>
-      <c r="D247" s="145">
+      <c r="D247" s="139">
         <f t="shared" si="34"/>
         <v>2000</v>
       </c>
       <c r="F247" s="7"/>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A248" s="139" t="s">
+      <c r="A248" s="133" t="s">
         <v>116</v>
       </c>
-      <c r="B248" s="144">
+      <c r="B248" s="138">
         <v>2</v>
       </c>
-      <c r="C248" s="145">
+      <c r="C248" s="139">
         <v>400</v>
       </c>
-      <c r="D248" s="145">
+      <c r="D248" s="139">
         <f t="shared" si="34"/>
         <v>800</v>
       </c>
       <c r="F248" s="7"/>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A249" s="139" t="s">
+      <c r="A249" s="133" t="s">
         <v>112</v>
       </c>
-      <c r="B249" s="144">
-        <v>0</v>
-      </c>
-      <c r="C249" s="145">
+      <c r="B249" s="138">
+        <v>0</v>
+      </c>
+      <c r="C249" s="139">
         <v>2500</v>
       </c>
-      <c r="D249" s="145">
+      <c r="D249" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F249" s="7"/>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A250" s="149" t="s">
+      <c r="A250" s="143" t="s">
         <v>111</v>
       </c>
-      <c r="B250" s="144">
-        <v>0</v>
-      </c>
-      <c r="C250" s="145">
+      <c r="B250" s="138">
+        <v>0</v>
+      </c>
+      <c r="C250" s="139">
         <v>2000</v>
       </c>
-      <c r="D250" s="145">
+      <c r="D250" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F250" s="7"/>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A251" s="139" t="s">
+      <c r="A251" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="B251" s="144">
-        <v>1</v>
-      </c>
-      <c r="C251" s="145">
+      <c r="B251" s="138">
+        <v>1</v>
+      </c>
+      <c r="C251" s="139">
         <v>5000</v>
       </c>
-      <c r="D251" s="145">
+      <c r="D251" s="139">
         <f t="shared" si="34"/>
         <v>5000</v>
       </c>
       <c r="F251" s="7"/>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A252" s="139" t="s">
+      <c r="A252" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="B252" s="144">
-        <v>1</v>
-      </c>
-      <c r="C252" s="145">
+      <c r="B252" s="138">
+        <v>1</v>
+      </c>
+      <c r="C252" s="139">
         <v>1000</v>
       </c>
-      <c r="D252" s="145">
+      <c r="D252" s="139">
         <f t="shared" si="34"/>
         <v>1000</v>
       </c>
       <c r="F252" s="7"/>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A253" s="139" t="s">
+      <c r="A253" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="B253" s="144">
+      <c r="B253" s="138">
         <v>0.05</v>
       </c>
-      <c r="C253" s="145">
+      <c r="C253" s="139">
         <v>8000</v>
       </c>
-      <c r="D253" s="145">
+      <c r="D253" s="139">
         <f t="shared" si="34"/>
         <v>400</v>
       </c>
       <c r="F253" s="7"/>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A254" s="139" t="s">
+      <c r="A254" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="B254" s="144">
+      <c r="B254" s="138">
         <v>2</v>
       </c>
-      <c r="C254" s="145">
+      <c r="C254" s="139">
         <v>400</v>
       </c>
-      <c r="D254" s="145">
+      <c r="D254" s="139">
         <f t="shared" si="34"/>
         <v>800</v>
       </c>
       <c r="F254" s="7"/>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A255" s="139" t="s">
+      <c r="A255" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="B255" s="144">
+      <c r="B255" s="138">
         <v>0.1</v>
       </c>
-      <c r="C255" s="145">
+      <c r="C255" s="139">
         <v>500</v>
       </c>
-      <c r="D255" s="145">
+      <c r="D255" s="139">
         <f t="shared" si="34"/>
         <v>50</v>
       </c>
       <c r="F255" s="7"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A256" s="139" t="s">
+      <c r="A256" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="B256" s="144">
+      <c r="B256" s="138">
         <v>0.5</v>
       </c>
-      <c r="C256" s="145">
+      <c r="C256" s="139">
         <v>500</v>
       </c>
-      <c r="D256" s="145">
+      <c r="D256" s="139">
         <f t="shared" si="34"/>
         <v>250</v>
       </c>
       <c r="F256" s="7"/>
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A257" s="139" t="s">
+      <c r="A257" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="B257" s="144">
+      <c r="B257" s="138">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="C257" s="145">
+      <c r="C257" s="139">
         <v>1500</v>
       </c>
-      <c r="D257" s="145">
+      <c r="D257" s="139">
         <f t="shared" si="34"/>
         <v>25</v>
       </c>
       <c r="F257" s="7"/>
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A258" s="136"/>
-      <c r="B258" s="136"/>
-      <c r="C258" s="136"/>
-      <c r="D258" s="150"/>
+      <c r="A258" s="130"/>
+      <c r="B258" s="130"/>
+      <c r="C258" s="130"/>
+      <c r="D258" s="144"/>
       <c r="F258" s="7"/>
     </row>
     <row r="259" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="141" t="s">
+      <c r="A259" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B259" s="151"/>
-      <c r="C259" s="141"/>
-      <c r="D259" s="151">
+      <c r="B259" s="145"/>
+      <c r="C259" s="135"/>
+      <c r="D259" s="145">
         <f>SUM(D243:D258)</f>
         <v>11125</v>
       </c>
       <c r="F259" s="7"/>
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A260" s="136"/>
-      <c r="B260" s="150"/>
-      <c r="C260" s="140">
+      <c r="A260" s="130"/>
+      <c r="B260" s="144"/>
+      <c r="C260" s="134">
         <f>+$B$102*B270</f>
         <v>304000</v>
       </c>
-      <c r="D260" s="150"/>
+      <c r="D260" s="144"/>
       <c r="F260" s="7"/>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
@@ -8085,42 +8150,42 @@
       <c r="G285" s="15"/>
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A286" s="135" t="s">
+      <c r="A286" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="B286" s="136"/>
-      <c r="C286" s="136"/>
+      <c r="B286" s="130"/>
+      <c r="C286" s="130"/>
       <c r="F286" s="47"/>
       <c r="G286" s="15"/>
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A287" s="137"/>
-      <c r="B287" s="137"/>
-      <c r="C287" s="136"/>
+      <c r="A287" s="131"/>
+      <c r="B287" s="131"/>
+      <c r="C287" s="130"/>
       <c r="F287" s="47"/>
       <c r="G287" s="15"/>
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A288" s="138" t="s">
+      <c r="A288" s="132" t="s">
         <v>85</v>
       </c>
-      <c r="B288" s="138" t="s">
+      <c r="B288" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="C288" s="138" t="s">
+      <c r="C288" s="132" t="s">
         <v>87</v>
       </c>
       <c r="F288" s="47"/>
       <c r="G288" s="15"/>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A289" s="139" t="s">
+      <c r="A289" s="133" t="s">
         <v>88</v>
       </c>
-      <c r="B289" s="140">
+      <c r="B289" s="134">
         <v>2388262</v>
       </c>
-      <c r="C289" s="140">
+      <c r="C289" s="134">
         <f>B289/$E$4/B$3</f>
         <v>1990.2183333333332</v>
       </c>
@@ -8128,13 +8193,13 @@
       <c r="G289" s="15"/>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A290" s="139" t="s">
+      <c r="A290" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="B290" s="140">
+      <c r="B290" s="134">
         <v>6775276.5</v>
       </c>
-      <c r="C290" s="140">
+      <c r="C290" s="134">
         <f t="shared" ref="C290:C293" si="37">B290/$E$4/B$3</f>
         <v>5646.0637500000003</v>
       </c>
@@ -8142,26 +8207,26 @@
       <c r="G290" s="15"/>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A291" s="139" t="s">
+      <c r="A291" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="B291" s="140">
+      <c r="B291" s="134">
         <v>4783964.3999999994</v>
       </c>
-      <c r="C291" s="140">
+      <c r="C291" s="134">
         <f t="shared" si="37"/>
         <v>3986.6369999999997</v>
       </c>
       <c r="G291" s="15"/>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A292" s="139" t="s">
+      <c r="A292" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="B292" s="140">
+      <c r="B292" s="134">
         <v>6688000</v>
       </c>
-      <c r="C292" s="140">
+      <c r="C292" s="134">
         <f t="shared" si="37"/>
         <v>5573.333333333333</v>
       </c>
@@ -8170,143 +8235,143 @@
       <c r="G292" s="15"/>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A293" s="139" t="s">
+      <c r="A293" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="B293" s="140">
+      <c r="B293" s="134">
         <v>63000</v>
       </c>
-      <c r="C293" s="140">
+      <c r="C293" s="134">
         <f t="shared" si="37"/>
         <v>52.5</v>
       </c>
       <c r="G293" s="15"/>
     </row>
     <row r="294" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="141" t="s">
+      <c r="A294" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B294" s="141"/>
-      <c r="C294" s="142">
+      <c r="B294" s="135"/>
+      <c r="C294" s="136">
         <f>SUM(C289:C293)</f>
         <v>17248.752416666666</v>
       </c>
       <c r="G294" s="15"/>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A296" s="135" t="s">
+      <c r="A296" s="129" t="s">
         <v>128</v>
       </c>
-      <c r="B296" s="136"/>
-      <c r="C296" s="136"/>
-      <c r="D296" s="136"/>
+      <c r="B296" s="130"/>
+      <c r="C296" s="130"/>
+      <c r="D296" s="130"/>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A297" s="136"/>
-      <c r="B297" s="136"/>
-      <c r="C297" s="136"/>
-      <c r="D297" s="136"/>
+      <c r="A297" s="130"/>
+      <c r="B297" s="130"/>
+      <c r="C297" s="130"/>
+      <c r="D297" s="130"/>
       <c r="H297" s="37"/>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A298" s="136"/>
-      <c r="B298" s="143" t="s">
+      <c r="A298" s="130"/>
+      <c r="B298" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C298" s="143" t="s">
+      <c r="C298" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D298" s="143" t="s">
+      <c r="D298" s="137" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A299" s="139" t="s">
+      <c r="A299" s="133" t="s">
         <v>117</v>
       </c>
-      <c r="B299" s="144">
-        <v>1</v>
-      </c>
-      <c r="C299" s="145">
+      <c r="B299" s="138">
+        <v>1</v>
+      </c>
+      <c r="C299" s="139">
         <v>10000000</v>
       </c>
-      <c r="D299" s="145">
+      <c r="D299" s="139">
         <f t="shared" ref="D299:D309" si="38">B299*C299</f>
         <v>10000000</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A300" s="139" t="s">
+      <c r="A300" s="133" t="s">
         <v>118</v>
       </c>
-      <c r="B300" s="144">
+      <c r="B300" s="138">
         <v>12</v>
       </c>
-      <c r="C300" s="145">
+      <c r="C300" s="139">
         <v>4000000</v>
       </c>
-      <c r="D300" s="145">
+      <c r="D300" s="139">
         <f t="shared" si="38"/>
         <v>48000000</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A301" s="139" t="s">
+      <c r="A301" s="133" t="s">
         <v>119</v>
       </c>
-      <c r="B301" s="144">
+      <c r="B301" s="138">
         <v>6</v>
       </c>
-      <c r="C301" s="145">
+      <c r="C301" s="139">
         <v>1000000</v>
       </c>
-      <c r="D301" s="145">
+      <c r="D301" s="139">
         <f t="shared" si="38"/>
         <v>6000000</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A302" s="139" t="s">
+      <c r="A302" s="133" t="s">
         <v>120</v>
       </c>
-      <c r="B302" s="144">
-        <v>1</v>
-      </c>
-      <c r="C302" s="145">
+      <c r="B302" s="138">
+        <v>1</v>
+      </c>
+      <c r="C302" s="139">
         <v>1000000</v>
       </c>
-      <c r="D302" s="145">
+      <c r="D302" s="139">
         <f t="shared" si="38"/>
         <v>1000000</v>
       </c>
       <c r="I302" s="37"/>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A303" s="139" t="s">
+      <c r="A303" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="B303" s="144">
+      <c r="B303" s="138">
         <v>6</v>
       </c>
-      <c r="C303" s="145">
+      <c r="C303" s="139">
         <v>2000000</v>
       </c>
-      <c r="D303" s="145">
+      <c r="D303" s="139">
         <f t="shared" si="38"/>
         <v>12000000</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A304" s="139" t="s">
+      <c r="A304" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="B304" s="144">
+      <c r="B304" s="138">
         <v>3</v>
       </c>
-      <c r="C304" s="145">
+      <c r="C304" s="139">
         <v>2500000</v>
       </c>
-      <c r="D304" s="145">
+      <c r="D304" s="139">
         <f t="shared" si="38"/>
         <v>7500000</v>
       </c>
@@ -8314,116 +8379,116 @@
       <c r="G304" s="27"/>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A305" s="139" t="s">
+      <c r="A305" s="133" t="s">
         <v>123</v>
       </c>
-      <c r="B305" s="144">
+      <c r="B305" s="138">
         <v>10</v>
       </c>
-      <c r="C305" s="145">
+      <c r="C305" s="139">
         <v>400000</v>
       </c>
-      <c r="D305" s="145">
+      <c r="D305" s="139">
         <f t="shared" si="38"/>
         <v>4000000</v>
       </c>
       <c r="G305" s="29"/>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A306" s="139" t="s">
+      <c r="A306" s="133" t="s">
         <v>124</v>
       </c>
-      <c r="B306" s="144">
-        <v>1</v>
-      </c>
-      <c r="C306" s="145">
+      <c r="B306" s="138">
+        <v>1</v>
+      </c>
+      <c r="C306" s="139">
         <v>5000000</v>
       </c>
-      <c r="D306" s="145">
+      <c r="D306" s="139">
         <f t="shared" si="38"/>
         <v>5000000</v>
       </c>
       <c r="H306" s="30"/>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A307" s="139" t="s">
+      <c r="A307" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B307" s="144">
+      <c r="B307" s="138">
         <v>2</v>
       </c>
-      <c r="C307" s="145">
+      <c r="C307" s="139">
         <v>2000000</v>
       </c>
-      <c r="D307" s="145">
+      <c r="D307" s="139">
         <f t="shared" si="38"/>
         <v>4000000</v>
       </c>
       <c r="H307" s="29"/>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A308" s="139" t="s">
+      <c r="A308" s="133" t="s">
         <v>126</v>
       </c>
-      <c r="B308" s="144">
+      <c r="B308" s="138">
         <v>5</v>
       </c>
-      <c r="C308" s="145">
+      <c r="C308" s="139">
         <v>400000</v>
       </c>
-      <c r="D308" s="145">
+      <c r="D308" s="139">
         <f t="shared" si="38"/>
         <v>2000000</v>
       </c>
       <c r="H308" s="29"/>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A309" s="139" t="s">
+      <c r="A309" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="B309" s="144">
-        <v>1</v>
-      </c>
-      <c r="C309" s="145">
+      <c r="B309" s="138">
+        <v>1</v>
+      </c>
+      <c r="C309" s="139">
         <v>10000000</v>
       </c>
-      <c r="D309" s="145">
+      <c r="D309" s="139">
         <f t="shared" si="38"/>
         <v>10000000</v>
       </c>
       <c r="H309" s="29"/>
     </row>
     <row r="310" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="141" t="s">
+      <c r="A310" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B310" s="141"/>
-      <c r="C310" s="141"/>
-      <c r="D310" s="146">
+      <c r="B310" s="135"/>
+      <c r="C310" s="135"/>
+      <c r="D310" s="140">
         <f>SUM(D299:D309)</f>
         <v>109500000</v>
       </c>
       <c r="H310" s="29"/>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A311" s="136" t="s">
+      <c r="A311" s="130" t="s">
         <v>129</v>
       </c>
-      <c r="B311" s="136"/>
-      <c r="C311" s="136"/>
-      <c r="D311" s="147">
+      <c r="B311" s="130"/>
+      <c r="C311" s="130"/>
+      <c r="D311" s="141">
         <f>D310/12</f>
         <v>9125000</v>
       </c>
       <c r="H311" s="29"/>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A312" s="136" t="s">
+      <c r="A312" s="130" t="s">
         <v>138</v>
       </c>
-      <c r="B312" s="136"/>
-      <c r="C312" s="136"/>
-      <c r="D312" s="147">
+      <c r="B312" s="130"/>
+      <c r="C312" s="130"/>
+      <c r="D312" s="141">
         <f>D311/B3</f>
         <v>2281250</v>
       </c>
@@ -8431,12 +8496,12 @@
       <c r="I312" s="30"/>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A313" s="136" t="s">
+      <c r="A313" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="B313" s="136"/>
-      <c r="C313" s="136"/>
-      <c r="D313" s="147">
+      <c r="B313" s="130"/>
+      <c r="C313" s="130"/>
+      <c r="D313" s="141">
         <f>D312/D161</f>
         <v>7604.166666666667</v>
       </c>
@@ -8536,6 +8601,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11564,12 +11630,12 @@
         <f>B126/$E$4/B$3</f>
         <v>1990.2183333333332</v>
       </c>
-      <c r="D126" s="129" t="s">
+      <c r="D126" s="146" t="s">
         <v>224</v>
       </c>
-      <c r="E126" s="130"/>
-      <c r="F126" s="130"/>
-      <c r="G126" s="130"/>
+      <c r="E126" s="147"/>
+      <c r="F126" s="147"/>
+      <c r="G126" s="147"/>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" s="115" t="s">
@@ -11884,18 +11950,18 @@
       <c r="D154" s="34"/>
     </row>
     <row r="155" spans="1:4" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="131" t="s">
+      <c r="A155" s="148" t="s">
         <v>225</v>
       </c>
-      <c r="B155" s="131"/>
-      <c r="C155" s="131"/>
-      <c r="D155" s="131"/>
+      <c r="B155" s="148"/>
+      <c r="C155" s="148"/>
+      <c r="D155" s="148"/>
     </row>
     <row r="156" spans="1:4" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="131"/>
-      <c r="B156" s="131"/>
-      <c r="C156" s="131"/>
-      <c r="D156" s="131"/>
+      <c r="A156" s="148"/>
+      <c r="B156" s="148"/>
+      <c r="C156" s="148"/>
+      <c r="D156" s="148"/>
     </row>
     <row r="157" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="158" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -13893,131 +13959,131 @@
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A229" s="135" t="s">
+      <c r="A229" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="B229" s="136"/>
-      <c r="C229" s="136"/>
-      <c r="D229" s="136"/>
+      <c r="B229" s="130"/>
+      <c r="C229" s="130"/>
+      <c r="D229" s="130"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="136"/>
-      <c r="B230" s="136"/>
-      <c r="C230" s="136"/>
-      <c r="D230" s="136"/>
+      <c r="A230" s="130"/>
+      <c r="B230" s="130"/>
+      <c r="C230" s="130"/>
+      <c r="D230" s="130"/>
       <c r="F230" s="7"/>
     </row>
     <row r="231" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="143" t="s">
+      <c r="A231" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="B231" s="143" t="s">
+      <c r="B231" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C231" s="143" t="s">
+      <c r="C231" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D231" s="143" t="s">
+      <c r="D231" s="137" t="s">
         <v>34</v>
       </c>
       <c r="F231" s="7"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A232" s="139" t="s">
+      <c r="A232" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="B232" s="144">
-        <v>0</v>
-      </c>
-      <c r="C232" s="145">
+      <c r="B232" s="138">
+        <v>0</v>
+      </c>
+      <c r="C232" s="139">
         <v>9000</v>
       </c>
-      <c r="D232" s="139">
+      <c r="D232" s="133">
         <f>C232*B232</f>
         <v>0</v>
       </c>
       <c r="F232" s="7"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A233" s="139" t="s">
+      <c r="A233" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="B233" s="144">
-        <v>1</v>
-      </c>
-      <c r="C233" s="145">
+      <c r="B233" s="138">
+        <v>1</v>
+      </c>
+      <c r="C233" s="139">
         <v>1000</v>
       </c>
-      <c r="D233" s="139">
+      <c r="D233" s="133">
         <f t="shared" ref="D233:D236" si="33">C233*B233</f>
         <v>1000</v>
       </c>
       <c r="F233" s="7"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A234" s="139" t="s">
+      <c r="A234" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="B234" s="144">
-        <v>0</v>
-      </c>
-      <c r="C234" s="145">
+      <c r="B234" s="138">
+        <v>0</v>
+      </c>
+      <c r="C234" s="139">
         <v>1200</v>
       </c>
-      <c r="D234" s="139">
+      <c r="D234" s="133">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F234" s="7"/>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A235" s="139" t="s">
+      <c r="A235" s="133" t="s">
         <v>44</v>
       </c>
-      <c r="B235" s="144">
+      <c r="B235" s="138">
         <f>1/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C235" s="145">
+      <c r="C235" s="139">
         <v>70479</v>
       </c>
-      <c r="D235" s="139">
+      <c r="D235" s="133">
         <f t="shared" si="33"/>
         <v>352.39499999999998</v>
       </c>
       <c r="F235" s="7"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A236" s="139" t="s">
+      <c r="A236" s="133" t="s">
         <v>45</v>
       </c>
-      <c r="B236" s="144">
+      <c r="B236" s="138">
         <f>1/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C236" s="145">
+      <c r="C236" s="139">
         <v>55000</v>
       </c>
-      <c r="D236" s="139">
+      <c r="D236" s="133">
         <f t="shared" si="33"/>
         <v>275</v>
       </c>
       <c r="F236" s="7"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A237" s="136"/>
-      <c r="B237" s="148"/>
-      <c r="C237" s="136"/>
-      <c r="D237" s="136"/>
+      <c r="A237" s="130"/>
+      <c r="B237" s="142"/>
+      <c r="C237" s="130"/>
+      <c r="D237" s="130"/>
       <c r="F237" s="7"/>
     </row>
     <row r="238" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="141" t="s">
+      <c r="A238" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B238" s="151"/>
-      <c r="C238" s="141"/>
-      <c r="D238" s="151">
+      <c r="B238" s="145"/>
+      <c r="C238" s="135"/>
+      <c r="D238" s="145">
         <f>SUM(D232:D237)</f>
         <v>1627.395</v>
       </c>
@@ -14029,304 +14095,304 @@
       <c r="F239" s="7"/>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A240" s="135" t="s">
+      <c r="A240" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="B240" s="148"/>
-      <c r="C240" s="136"/>
-      <c r="D240" s="136"/>
+      <c r="B240" s="142"/>
+      <c r="C240" s="130"/>
+      <c r="D240" s="130"/>
       <c r="F240" s="7"/>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A241" s="135"/>
-      <c r="B241" s="148"/>
-      <c r="C241" s="136"/>
-      <c r="D241" s="136"/>
+      <c r="A241" s="129"/>
+      <c r="B241" s="142"/>
+      <c r="C241" s="130"/>
+      <c r="D241" s="130"/>
       <c r="F241" s="7"/>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A242" s="143" t="s">
+      <c r="A242" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="B242" s="143" t="s">
+      <c r="B242" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C242" s="143" t="s">
+      <c r="C242" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D242" s="143" t="s">
+      <c r="D242" s="137" t="s">
         <v>34</v>
       </c>
       <c r="F242" s="7"/>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A243" s="139" t="s">
+      <c r="A243" s="133" t="s">
         <v>110</v>
       </c>
-      <c r="B243" s="144">
-        <v>1</v>
-      </c>
-      <c r="C243" s="145">
+      <c r="B243" s="138">
+        <v>1</v>
+      </c>
+      <c r="C243" s="139">
         <v>400</v>
       </c>
-      <c r="D243" s="145">
+      <c r="D243" s="139">
         <f t="shared" ref="D243:D257" si="34">B243*C243</f>
         <v>400</v>
       </c>
       <c r="F243" s="7"/>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A244" s="139" t="s">
+      <c r="A244" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="B244" s="144">
-        <v>1</v>
-      </c>
-      <c r="C244" s="145">
+      <c r="B244" s="138">
+        <v>1</v>
+      </c>
+      <c r="C244" s="139">
         <v>400</v>
       </c>
-      <c r="D244" s="145">
+      <c r="D244" s="139">
         <f t="shared" si="34"/>
         <v>400</v>
       </c>
       <c r="F244" s="7"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A245" s="139" t="s">
+      <c r="A245" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="B245" s="144">
-        <v>0</v>
-      </c>
-      <c r="C245" s="145">
+      <c r="B245" s="138">
+        <v>0</v>
+      </c>
+      <c r="C245" s="139">
         <v>400</v>
       </c>
-      <c r="D245" s="145">
+      <c r="D245" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F245" s="7"/>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A246" s="139" t="s">
+      <c r="A246" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="B246" s="144">
-        <v>0</v>
-      </c>
-      <c r="C246" s="145">
+      <c r="B246" s="138">
+        <v>0</v>
+      </c>
+      <c r="C246" s="139">
         <v>500</v>
       </c>
-      <c r="D246" s="145">
+      <c r="D246" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F246" s="7"/>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A247" s="139" t="s">
+      <c r="A247" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="B247" s="144">
-        <v>1</v>
-      </c>
-      <c r="C247" s="145">
+      <c r="B247" s="138">
+        <v>1</v>
+      </c>
+      <c r="C247" s="139">
         <v>2000</v>
       </c>
-      <c r="D247" s="145">
+      <c r="D247" s="139">
         <f t="shared" si="34"/>
         <v>2000</v>
       </c>
       <c r="F247" s="7"/>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A248" s="139" t="s">
+      <c r="A248" s="133" t="s">
         <v>116</v>
       </c>
-      <c r="B248" s="144">
+      <c r="B248" s="138">
         <v>2</v>
       </c>
-      <c r="C248" s="145">
+      <c r="C248" s="139">
         <v>400</v>
       </c>
-      <c r="D248" s="145">
+      <c r="D248" s="139">
         <f t="shared" si="34"/>
         <v>800</v>
       </c>
       <c r="F248" s="7"/>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A249" s="139" t="s">
+      <c r="A249" s="133" t="s">
         <v>112</v>
       </c>
-      <c r="B249" s="144">
-        <v>0</v>
-      </c>
-      <c r="C249" s="145">
+      <c r="B249" s="138">
+        <v>0</v>
+      </c>
+      <c r="C249" s="139">
         <v>2500</v>
       </c>
-      <c r="D249" s="145">
+      <c r="D249" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F249" s="7"/>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A250" s="149" t="s">
+      <c r="A250" s="143" t="s">
         <v>111</v>
       </c>
-      <c r="B250" s="144">
-        <v>0</v>
-      </c>
-      <c r="C250" s="145">
+      <c r="B250" s="138">
+        <v>0</v>
+      </c>
+      <c r="C250" s="139">
         <v>2000</v>
       </c>
-      <c r="D250" s="145">
+      <c r="D250" s="139">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="F250" s="7"/>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A251" s="139" t="s">
+      <c r="A251" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="B251" s="144">
-        <v>1</v>
-      </c>
-      <c r="C251" s="145">
+      <c r="B251" s="138">
+        <v>1</v>
+      </c>
+      <c r="C251" s="139">
         <v>5000</v>
       </c>
-      <c r="D251" s="145">
+      <c r="D251" s="139">
         <f t="shared" si="34"/>
         <v>5000</v>
       </c>
       <c r="F251" s="7"/>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A252" s="139" t="s">
+      <c r="A252" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="B252" s="144">
-        <v>1</v>
-      </c>
-      <c r="C252" s="145">
+      <c r="B252" s="138">
+        <v>1</v>
+      </c>
+      <c r="C252" s="139">
         <v>1000</v>
       </c>
-      <c r="D252" s="145">
+      <c r="D252" s="139">
         <f t="shared" si="34"/>
         <v>1000</v>
       </c>
       <c r="F252" s="7"/>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A253" s="139" t="s">
+      <c r="A253" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="B253" s="144">
+      <c r="B253" s="138">
         <v>0.05</v>
       </c>
-      <c r="C253" s="145">
+      <c r="C253" s="139">
         <v>8000</v>
       </c>
-      <c r="D253" s="145">
+      <c r="D253" s="139">
         <f t="shared" si="34"/>
         <v>400</v>
       </c>
       <c r="F253" s="7"/>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A254" s="139" t="s">
+      <c r="A254" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="B254" s="144">
+      <c r="B254" s="138">
         <v>2</v>
       </c>
-      <c r="C254" s="145">
+      <c r="C254" s="139">
         <v>400</v>
       </c>
-      <c r="D254" s="145">
+      <c r="D254" s="139">
         <f t="shared" si="34"/>
         <v>800</v>
       </c>
       <c r="F254" s="7"/>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A255" s="139" t="s">
+      <c r="A255" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="B255" s="144">
+      <c r="B255" s="138">
         <v>0.1</v>
       </c>
-      <c r="C255" s="145">
+      <c r="C255" s="139">
         <v>500</v>
       </c>
-      <c r="D255" s="145">
+      <c r="D255" s="139">
         <f t="shared" si="34"/>
         <v>50</v>
       </c>
       <c r="F255" s="7"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A256" s="139" t="s">
+      <c r="A256" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="B256" s="144">
+      <c r="B256" s="138">
         <v>0.5</v>
       </c>
-      <c r="C256" s="145">
+      <c r="C256" s="139">
         <v>500</v>
       </c>
-      <c r="D256" s="145">
+      <c r="D256" s="139">
         <f t="shared" si="34"/>
         <v>250</v>
       </c>
       <c r="F256" s="7"/>
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A257" s="139" t="s">
+      <c r="A257" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="B257" s="144">
+      <c r="B257" s="138">
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="C257" s="145">
+      <c r="C257" s="139">
         <v>1500</v>
       </c>
-      <c r="D257" s="145">
+      <c r="D257" s="139">
         <f t="shared" si="34"/>
         <v>25</v>
       </c>
       <c r="F257" s="7"/>
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A258" s="136"/>
-      <c r="B258" s="136"/>
-      <c r="C258" s="136"/>
-      <c r="D258" s="150"/>
+      <c r="A258" s="130"/>
+      <c r="B258" s="130"/>
+      <c r="C258" s="130"/>
+      <c r="D258" s="144"/>
       <c r="F258" s="7"/>
     </row>
     <row r="259" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="141" t="s">
+      <c r="A259" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B259" s="151"/>
-      <c r="C259" s="141"/>
-      <c r="D259" s="151">
+      <c r="B259" s="145"/>
+      <c r="C259" s="135"/>
+      <c r="D259" s="145">
         <f>SUM(D243:D258)</f>
         <v>11125</v>
       </c>
       <c r="F259" s="7"/>
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A260" s="136"/>
-      <c r="B260" s="150"/>
-      <c r="C260" s="140">
+      <c r="A260" s="130"/>
+      <c r="B260" s="144"/>
+      <c r="C260" s="134">
         <f>+$B$102*B270</f>
         <v>304000</v>
       </c>
-      <c r="D260" s="150"/>
+      <c r="D260" s="144"/>
       <c r="F260" s="7"/>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.2">
@@ -14827,42 +14893,42 @@
       <c r="G285" s="15"/>
     </row>
     <row r="286" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A286" s="135" t="s">
+      <c r="A286" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="B286" s="136"/>
-      <c r="C286" s="136"/>
+      <c r="B286" s="130"/>
+      <c r="C286" s="130"/>
       <c r="F286" s="47"/>
       <c r="G286" s="15"/>
     </row>
     <row r="287" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A287" s="137"/>
-      <c r="B287" s="137"/>
-      <c r="C287" s="136"/>
+      <c r="A287" s="131"/>
+      <c r="B287" s="131"/>
+      <c r="C287" s="130"/>
       <c r="F287" s="47"/>
       <c r="G287" s="15"/>
     </row>
     <row r="288" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A288" s="138" t="s">
+      <c r="A288" s="132" t="s">
         <v>85</v>
       </c>
-      <c r="B288" s="138" t="s">
+      <c r="B288" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="C288" s="138" t="s">
+      <c r="C288" s="132" t="s">
         <v>87</v>
       </c>
       <c r="F288" s="47"/>
       <c r="G288" s="15"/>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A289" s="139" t="s">
+      <c r="A289" s="133" t="s">
         <v>88</v>
       </c>
-      <c r="B289" s="140">
+      <c r="B289" s="134">
         <v>2388262</v>
       </c>
-      <c r="C289" s="140">
+      <c r="C289" s="134">
         <f>B289/$E$4/B$3</f>
         <v>1990.2183333333332</v>
       </c>
@@ -14870,13 +14936,13 @@
       <c r="G289" s="15"/>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A290" s="139" t="s">
+      <c r="A290" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="B290" s="140">
+      <c r="B290" s="134">
         <v>6775276.5</v>
       </c>
-      <c r="C290" s="140">
+      <c r="C290" s="134">
         <f t="shared" ref="C290:C293" si="37">B290/$E$4/B$3</f>
         <v>5646.0637500000003</v>
       </c>
@@ -14884,26 +14950,26 @@
       <c r="G290" s="15"/>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A291" s="139" t="s">
+      <c r="A291" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="B291" s="140">
+      <c r="B291" s="134">
         <v>4783964.3999999994</v>
       </c>
-      <c r="C291" s="140">
+      <c r="C291" s="134">
         <f t="shared" si="37"/>
         <v>3986.6369999999997</v>
       </c>
       <c r="G291" s="15"/>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A292" s="139" t="s">
+      <c r="A292" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="B292" s="140">
+      <c r="B292" s="134">
         <v>6688000</v>
       </c>
-      <c r="C292" s="140">
+      <c r="C292" s="134">
         <f t="shared" si="37"/>
         <v>5573.333333333333</v>
       </c>
@@ -14912,143 +14978,143 @@
       <c r="G292" s="15"/>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A293" s="139" t="s">
+      <c r="A293" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="B293" s="140">
+      <c r="B293" s="134">
         <v>63000</v>
       </c>
-      <c r="C293" s="140">
+      <c r="C293" s="134">
         <f t="shared" si="37"/>
         <v>52.5</v>
       </c>
       <c r="G293" s="15"/>
     </row>
     <row r="294" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="141" t="s">
+      <c r="A294" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B294" s="141"/>
-      <c r="C294" s="142">
+      <c r="B294" s="135"/>
+      <c r="C294" s="136">
         <f>SUM(C289:C293)</f>
         <v>17248.752416666666</v>
       </c>
       <c r="G294" s="15"/>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A296" s="135" t="s">
+      <c r="A296" s="129" t="s">
         <v>128</v>
       </c>
-      <c r="B296" s="136"/>
-      <c r="C296" s="136"/>
-      <c r="D296" s="136"/>
+      <c r="B296" s="130"/>
+      <c r="C296" s="130"/>
+      <c r="D296" s="130"/>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A297" s="136"/>
-      <c r="B297" s="136"/>
-      <c r="C297" s="136"/>
-      <c r="D297" s="136"/>
+      <c r="A297" s="130"/>
+      <c r="B297" s="130"/>
+      <c r="C297" s="130"/>
+      <c r="D297" s="130"/>
       <c r="H297" s="37"/>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A298" s="136"/>
-      <c r="B298" s="143" t="s">
+      <c r="A298" s="130"/>
+      <c r="B298" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C298" s="143" t="s">
+      <c r="C298" s="137" t="s">
         <v>33</v>
       </c>
-      <c r="D298" s="143" t="s">
+      <c r="D298" s="137" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A299" s="139" t="s">
+      <c r="A299" s="133" t="s">
         <v>117</v>
       </c>
-      <c r="B299" s="144">
-        <v>1</v>
-      </c>
-      <c r="C299" s="145">
+      <c r="B299" s="138">
+        <v>1</v>
+      </c>
+      <c r="C299" s="139">
         <v>10000000</v>
       </c>
-      <c r="D299" s="145">
+      <c r="D299" s="139">
         <f t="shared" ref="D299:D309" si="38">B299*C299</f>
         <v>10000000</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A300" s="139" t="s">
+      <c r="A300" s="133" t="s">
         <v>118</v>
       </c>
-      <c r="B300" s="144">
+      <c r="B300" s="138">
         <v>12</v>
       </c>
-      <c r="C300" s="145">
+      <c r="C300" s="139">
         <v>4000000</v>
       </c>
-      <c r="D300" s="145">
+      <c r="D300" s="139">
         <f t="shared" si="38"/>
         <v>48000000</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A301" s="139" t="s">
+      <c r="A301" s="133" t="s">
         <v>119</v>
       </c>
-      <c r="B301" s="144">
+      <c r="B301" s="138">
         <v>6</v>
       </c>
-      <c r="C301" s="145">
+      <c r="C301" s="139">
         <v>1000000</v>
       </c>
-      <c r="D301" s="145">
+      <c r="D301" s="139">
         <f t="shared" si="38"/>
         <v>6000000</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A302" s="139" t="s">
+      <c r="A302" s="133" t="s">
         <v>120</v>
       </c>
-      <c r="B302" s="144">
-        <v>1</v>
-      </c>
-      <c r="C302" s="145">
+      <c r="B302" s="138">
+        <v>1</v>
+      </c>
+      <c r="C302" s="139">
         <v>1000000</v>
       </c>
-      <c r="D302" s="145">
+      <c r="D302" s="139">
         <f t="shared" si="38"/>
         <v>1000000</v>
       </c>
       <c r="I302" s="37"/>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A303" s="139" t="s">
+      <c r="A303" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="B303" s="144">
+      <c r="B303" s="138">
         <v>6</v>
       </c>
-      <c r="C303" s="145">
+      <c r="C303" s="139">
         <v>2000000</v>
       </c>
-      <c r="D303" s="145">
+      <c r="D303" s="139">
         <f t="shared" si="38"/>
         <v>12000000</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A304" s="139" t="s">
+      <c r="A304" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="B304" s="144">
+      <c r="B304" s="138">
         <v>3</v>
       </c>
-      <c r="C304" s="145">
+      <c r="C304" s="139">
         <v>2500000</v>
       </c>
-      <c r="D304" s="145">
+      <c r="D304" s="139">
         <f t="shared" si="38"/>
         <v>7500000</v>
       </c>
@@ -15056,116 +15122,116 @@
       <c r="G304" s="27"/>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A305" s="139" t="s">
+      <c r="A305" s="133" t="s">
         <v>123</v>
       </c>
-      <c r="B305" s="144">
+      <c r="B305" s="138">
         <v>10</v>
       </c>
-      <c r="C305" s="145">
+      <c r="C305" s="139">
         <v>400000</v>
       </c>
-      <c r="D305" s="145">
+      <c r="D305" s="139">
         <f t="shared" si="38"/>
         <v>4000000</v>
       </c>
       <c r="G305" s="29"/>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A306" s="139" t="s">
+      <c r="A306" s="133" t="s">
         <v>124</v>
       </c>
-      <c r="B306" s="144">
-        <v>1</v>
-      </c>
-      <c r="C306" s="145">
+      <c r="B306" s="138">
+        <v>1</v>
+      </c>
+      <c r="C306" s="139">
         <v>5000000</v>
       </c>
-      <c r="D306" s="145">
+      <c r="D306" s="139">
         <f t="shared" si="38"/>
         <v>5000000</v>
       </c>
       <c r="H306" s="30"/>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A307" s="139" t="s">
+      <c r="A307" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B307" s="144">
+      <c r="B307" s="138">
         <v>2</v>
       </c>
-      <c r="C307" s="145">
+      <c r="C307" s="139">
         <v>2000000</v>
       </c>
-      <c r="D307" s="145">
+      <c r="D307" s="139">
         <f t="shared" si="38"/>
         <v>4000000</v>
       </c>
       <c r="H307" s="29"/>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A308" s="139" t="s">
+      <c r="A308" s="133" t="s">
         <v>126</v>
       </c>
-      <c r="B308" s="144">
+      <c r="B308" s="138">
         <v>5</v>
       </c>
-      <c r="C308" s="145">
+      <c r="C308" s="139">
         <v>400000</v>
       </c>
-      <c r="D308" s="145">
+      <c r="D308" s="139">
         <f t="shared" si="38"/>
         <v>2000000</v>
       </c>
       <c r="H308" s="29"/>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A309" s="139" t="s">
+      <c r="A309" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="B309" s="144">
-        <v>1</v>
-      </c>
-      <c r="C309" s="145">
+      <c r="B309" s="138">
+        <v>1</v>
+      </c>
+      <c r="C309" s="139">
         <v>10000000</v>
       </c>
-      <c r="D309" s="145">
+      <c r="D309" s="139">
         <f t="shared" si="38"/>
         <v>10000000</v>
       </c>
       <c r="H309" s="29"/>
     </row>
     <row r="310" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="141" t="s">
+      <c r="A310" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B310" s="141"/>
-      <c r="C310" s="141"/>
-      <c r="D310" s="146">
+      <c r="B310" s="135"/>
+      <c r="C310" s="135"/>
+      <c r="D310" s="140">
         <f>SUM(D299:D309)</f>
         <v>109500000</v>
       </c>
       <c r="H310" s="29"/>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A311" s="136" t="s">
+      <c r="A311" s="130" t="s">
         <v>129</v>
       </c>
-      <c r="B311" s="136"/>
-      <c r="C311" s="136"/>
-      <c r="D311" s="147">
+      <c r="B311" s="130"/>
+      <c r="C311" s="130"/>
+      <c r="D311" s="141">
         <f>D310/12</f>
         <v>9125000</v>
       </c>
       <c r="H311" s="29"/>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A312" s="136" t="s">
+      <c r="A312" s="130" t="s">
         <v>138</v>
       </c>
-      <c r="B312" s="136"/>
-      <c r="C312" s="136"/>
-      <c r="D312" s="147">
+      <c r="B312" s="130"/>
+      <c r="C312" s="130"/>
+      <c r="D312" s="141">
         <f>D311/B3</f>
         <v>2281250</v>
       </c>
@@ -15173,12 +15239,12 @@
       <c r="I312" s="30"/>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A313" s="136" t="s">
+      <c r="A313" s="130" t="s">
         <v>140</v>
       </c>
-      <c r="B313" s="136"/>
-      <c r="C313" s="136"/>
-      <c r="D313" s="147">
+      <c r="B313" s="130"/>
+      <c r="C313" s="130"/>
+      <c r="D313" s="141">
         <f>D312/D161</f>
         <v>7604.166666666667</v>
       </c>
@@ -16239,23 +16305,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="151" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="149" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="D4" s="132" t="s">
+      <c r="B4" s="150"/>
+      <c r="D4" s="149" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="133"/>
+      <c r="E4" s="150"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="95" t="s">
@@ -16781,15 +16847,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="b819869a-5527-41f8-bf27-4fbef748067a">
@@ -16798,6 +16855,15 @@
     <TaxCatchAll xmlns="ec36c1b3-45c0-40c9-96d4-e57661e8d407" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17008,20 +17074,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{244463B3-A800-4DEA-BE06-2554ACC63119}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{683A8DC6-E796-4DA8-B834-97E70B707C60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="b819869a-5527-41f8-bf27-4fbef748067a"/>
     <ds:schemaRef ds:uri="ec36c1b3-45c0-40c9-96d4-e57661e8d407"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{244463B3-A800-4DEA-BE06-2554ACC63119}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>